<commit_message>
Employee Module and Client Module few test cases
</commit_message>
<xml_diff>
--- a/testData/sai_TestData.xlsx
+++ b/testData/sai_TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaikumarVeeramalla\OneDrive - Client Server Technology Solutions LLC\Desktop\BGC_Microservices_UI\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{5CD887BF-489A-4318-9209-8A178EE546F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{657727F8-CB43-418E-9F33-8294D085BD7A}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{5CD887BF-489A-4318-9209-8A178EE546F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{69BE5DF4-D0BF-4630-A0F8-F6E1EFF1E647}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16480" windowHeight="8070" xr2:uid="{BE9F246B-8A45-404C-B1CA-8CEF9DDF31FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16480" windowHeight="8070" activeTab="1" xr2:uid="{BE9F246B-8A45-404C-B1CA-8CEF9DDF31FD}"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmployee" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCandidate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>EmpName</t>
   </si>
@@ -70,6 +71,27 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Auto Test</t>
+  </si>
+  <si>
+    <t>autotest</t>
+  </si>
+  <si>
+    <t>c@gmail.com</t>
+  </si>
+  <si>
+    <t>AutoinvalidTest123</t>
+  </si>
+  <si>
+    <t>3@gmail</t>
   </si>
 </sst>
 </file>
@@ -459,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8F81C5-FB7D-4927-B7C4-63D1AE7BB791}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,7 +596,90 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FAC199-8417-4604-814C-15ABB60CA164}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>19091997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>78</v>
+      </c>
+      <c r="E3">
+        <v>882323098</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D006247E-B821-4A20-9D78-74192A4BE261}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{2CBCC9CA-859C-4DB3-B00E-23F77E84ED66}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc374b43-8008-4bc9-911e-8bb9ac750c20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B324A40CAC669A4EA388FD165DA513B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2b45e0c43c51f5737c8d636c94a29f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dc374b43-8008-4bc9-911e-8bb9ac750c20" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5dc321c01f65b4c56c1fd44aacd0c552" ns3:_="">
     <xsd:import namespace="dc374b43-8008-4bc9-911e-8bb9ac750c20"/>
@@ -768,24 +873,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc374b43-8008-4bc9-911e-8bb9ac750c20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1832F7-29F7-44F2-A58C-5D9646608541}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc374b43-8008-4bc9-911e-8bb9ac750c20"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{778AAEC4-3862-48A0-B284-F96AFB9D1B3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFF4FE48-E58B-43B3-8664-265DA24B64C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -801,28 +913,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{778AAEC4-3862-48A0-B284-F96AFB9D1B3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1832F7-29F7-44F2-A58C-5D9646608541}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc374b43-8008-4bc9-911e-8bb9ac750c20"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
All Employee Test Scripts
</commit_message>
<xml_diff>
--- a/testData/sai_TestData.xlsx
+++ b/testData/sai_TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaikumarVeeramalla\OneDrive - Client Server Technology Solutions LLC\Desktop\BGC_Microservices_UI\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{5CD887BF-489A-4318-9209-8A178EE546F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{69BE5DF4-D0BF-4630-A0F8-F6E1EFF1E647}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{5CD887BF-489A-4318-9209-8A178EE546F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8FF0FEB0-C0A9-46D2-8236-63234CFF2393}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16480" windowHeight="8070" activeTab="1" xr2:uid="{BE9F246B-8A45-404C-B1CA-8CEF9DDF31FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16480" windowHeight="8070" activeTab="2" xr2:uid="{BE9F246B-8A45-404C-B1CA-8CEF9DDF31FD}"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmployee" sheetId="1" r:id="rId1"/>
     <sheet name="AddCandidate" sheetId="2" r:id="rId2"/>
+    <sheet name="Employee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>EmpName</t>
   </si>
@@ -92,6 +93,33 @@
   </si>
   <si>
     <t>3@gmail</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Father Name</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>T-13 Nandavanam colony</t>
+  </si>
+  <si>
+    <t>Ravinder</t>
+  </si>
+  <si>
+    <t>Saikumar Verramalla</t>
   </si>
 </sst>
 </file>
@@ -600,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FAC199-8417-4604-814C-15ABB60CA164}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -662,21 +690,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46A0082-6FFC-42CC-A95A-E6F2FE18CC42}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="34.90625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>2025</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc374b43-8008-4bc9-911e-8bb9ac750c20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc374b43-8008-4bc9-911e-8bb9ac750c20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -874,25 +957,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1832F7-29F7-44F2-A58C-5D9646608541}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc374b43-8008-4bc9-911e-8bb9ac750c20"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{778AAEC4-3862-48A0-B284-F96AFB9D1B3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE1832F7-29F7-44F2-A58C-5D9646608541}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc374b43-8008-4bc9-911e-8bb9ac750c20"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>